<commit_message>
NumMethods: passed lw3, lw5, lw6
</commit_message>
<xml_diff>
--- a/Numerical methods/LW3/LW3.xlsx
+++ b/Numerical methods/LW3/LW3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\studies\Numerical methods\LW3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\studies\Numerical methods\LW3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E3734A-5339-422C-BBC0-4A3F8723BC3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD55FA42-4A62-4843-B833-57C95BD93A1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8400" yWindow="3675" windowWidth="21585" windowHeight="11370" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Простой итерации" sheetId="1" r:id="rId1"/>
@@ -31,15 +31,12 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -61,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
   <si>
     <t>A_inf =</t>
   </si>
@@ -511,14 +508,14 @@
       <selection activeCell="S39" sqref="S39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="4" width="11.42578125" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" customWidth="1"/>
+    <col min="15" max="15" width="9.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:29" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
@@ -536,7 +533,7 @@
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
     </row>
-    <row r="2" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:29" x14ac:dyDescent="0.35">
       <c r="B2">
         <v>7.4980000000000002</v>
       </c>
@@ -591,7 +588,7 @@
         <v>11.872</v>
       </c>
     </row>
-    <row r="3" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:29" x14ac:dyDescent="0.35">
       <c r="B3">
         <v>-0.46700000000000003</v>
       </c>
@@ -646,7 +643,7 @@
         <v>11.920000000000002</v>
       </c>
     </row>
-    <row r="4" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:29" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>-0.90300000000000002</v>
       </c>
@@ -694,7 +691,7 @@
         <v>4.8899999999999997</v>
       </c>
     </row>
-    <row r="5" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:29" x14ac:dyDescent="0.35">
       <c r="B5">
         <v>0.56799999999999995</v>
       </c>
@@ -742,7 +739,7 @@
         <v>11.872</v>
       </c>
     </row>
-    <row r="6" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:29" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>0.751</v>
       </c>
@@ -790,7 +787,7 @@
         <v>11.510000000000002</v>
       </c>
     </row>
-    <row r="8" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:29" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -817,7 +814,7 @@
         <v>11.920000000000002</v>
       </c>
     </row>
-    <row r="12" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:29" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
@@ -847,7 +844,7 @@
       <c r="W12" s="2"/>
       <c r="X12" s="2"/>
     </row>
-    <row r="13" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:29" x14ac:dyDescent="0.35">
       <c r="B13">
         <v>1</v>
       </c>
@@ -926,7 +923,7 @@
         <v>12.872</v>
       </c>
     </row>
-    <row r="14" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:29" x14ac:dyDescent="0.35">
       <c r="B14">
         <v>0</v>
       </c>
@@ -1004,7 +1001,7 @@
         <v>12.920000000000002</v>
       </c>
     </row>
-    <row r="15" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:29" x14ac:dyDescent="0.35">
       <c r="B15">
         <v>0</v>
       </c>
@@ -1075,7 +1072,7 @@
         <v>5.89</v>
       </c>
     </row>
-    <row r="16" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:29" x14ac:dyDescent="0.35">
       <c r="B16">
         <v>0</v>
       </c>
@@ -1146,7 +1143,7 @@
         <v>12.872</v>
       </c>
     </row>
-    <row r="17" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:35" x14ac:dyDescent="0.35">
       <c r="B17">
         <v>0</v>
       </c>
@@ -1217,7 +1214,7 @@
         <v>12.510000000000002</v>
       </c>
     </row>
-    <row r="19" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:35" x14ac:dyDescent="0.35">
       <c r="T19">
         <f>SUM(T13:T17)</f>
         <v>9.1869999999999994</v>
@@ -1239,7 +1236,7 @@
         <v>12.920000000000002</v>
       </c>
     </row>
-    <row r="20" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:35" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>8</v>
       </c>
@@ -1247,7 +1244,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:35" x14ac:dyDescent="0.35">
       <c r="B21">
         <v>1</v>
       </c>
@@ -1276,7 +1273,7 @@
         <v>630001.31559298665</v>
       </c>
     </row>
-    <row r="22" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:35" x14ac:dyDescent="0.35">
       <c r="B22">
         <v>1</v>
       </c>
@@ -1299,7 +1296,7 @@
         <v>37.978260420282744</v>
       </c>
     </row>
-    <row r="23" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:35" x14ac:dyDescent="0.35">
       <c r="B23">
         <v>1</v>
       </c>
@@ -1322,7 +1319,7 @@
         <v>127.32641437190547</v>
       </c>
     </row>
-    <row r="24" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:35" x14ac:dyDescent="0.35">
       <c r="B24">
         <v>1</v>
       </c>
@@ -1345,7 +1342,7 @@
         <v>-45.445444911065273</v>
       </c>
     </row>
-    <row r="25" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:35" x14ac:dyDescent="0.35">
       <c r="B25">
         <v>1</v>
       </c>
@@ -1368,7 +1365,7 @@
         <v>30.252660722305784</v>
       </c>
     </row>
-    <row r="29" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:35" x14ac:dyDescent="0.35">
       <c r="B29" s="2" t="s">
         <v>5</v>
       </c>
@@ -1405,7 +1402,7 @@
       <c r="AC29" s="2"/>
       <c r="AD29" s="2"/>
     </row>
-    <row r="30" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:35" x14ac:dyDescent="0.35">
       <c r="B30">
         <v>1</v>
       </c>
@@ -1504,7 +1501,7 @@
         <v>0.84908389585342348</v>
       </c>
     </row>
-    <row r="31" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:35" x14ac:dyDescent="0.35">
       <c r="B31">
         <v>0</v>
       </c>
@@ -1602,7 +1599,7 @@
         <v>0.70329545181987152</v>
       </c>
     </row>
-    <row r="32" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:35" x14ac:dyDescent="0.35">
       <c r="B32">
         <v>0</v>
       </c>
@@ -1693,7 +1690,7 @@
         <v>0.82872101720269253</v>
       </c>
     </row>
-    <row r="33" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:32" x14ac:dyDescent="0.35">
       <c r="B33">
         <v>0</v>
       </c>
@@ -1784,7 +1781,7 @@
         <v>0.2697326203208556</v>
       </c>
     </row>
-    <row r="34" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:32" x14ac:dyDescent="0.35">
       <c r="B34">
         <v>0</v>
       </c>
@@ -1875,7 +1872,7 @@
         <v>0.22122015915119364</v>
       </c>
     </row>
-    <row r="36" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:32" x14ac:dyDescent="0.35">
       <c r="Z36">
         <f>SUM(Z30:Z34)</f>
         <v>0.70329545181987152</v>
@@ -1897,7 +1894,7 @@
         <v>0.67161080162229703</v>
       </c>
     </row>
-    <row r="37" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:32" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
         <v>12</v>
       </c>
@@ -1905,7 +1902,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:32" x14ac:dyDescent="0.35">
       <c r="B38">
         <v>1</v>
       </c>
@@ -1970,7 +1967,7 @@
         <v>-55.252000000000002</v>
       </c>
     </row>
-    <row r="39" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:32" x14ac:dyDescent="0.35">
       <c r="B39">
         <v>1</v>
       </c>
@@ -2020,7 +2017,7 @@
         <v>16.690761907804653</v>
       </c>
     </row>
-    <row r="40" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:32" x14ac:dyDescent="0.35">
       <c r="B40">
         <v>1</v>
       </c>
@@ -2070,7 +2067,7 @@
         <v>20.080044668961133</v>
       </c>
     </row>
-    <row r="41" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:32" x14ac:dyDescent="0.35">
       <c r="B41">
         <v>1</v>
       </c>
@@ -2120,7 +2117,7 @@
         <v>-78.561506490548851</v>
       </c>
     </row>
-    <row r="42" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:32" x14ac:dyDescent="0.35">
       <c r="B42">
         <v>1</v>
       </c>
@@ -2172,17 +2169,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="H12:L12"/>
+    <mergeCell ref="N12:R12"/>
     <mergeCell ref="Z29:AD29"/>
     <mergeCell ref="T12:X12"/>
     <mergeCell ref="B29:F29"/>
     <mergeCell ref="H29:L29"/>
     <mergeCell ref="N29:R29"/>
     <mergeCell ref="T29:X29"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="I1:N1"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="H12:L12"/>
-    <mergeCell ref="N12:R12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2191,18 +2188,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA0F3416-944A-40B7-BB96-2BB4AC54D766}">
-  <dimension ref="A1:AEY49"/>
+  <dimension ref="A1:AEY51"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>26</v>
       </c>
@@ -2226,7 +2223,7 @@
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
     </row>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B2">
         <v>5.2403000000000004</v>
       </c>
@@ -2276,7 +2273,7 @@
         <v>-2.5373000000000001</v>
       </c>
     </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B3">
         <v>-1.4360999999999999</v>
       </c>
@@ -2326,7 +2323,7 @@
         <v>2.5573000000000001</v>
       </c>
     </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>5.1886000000000001</v>
       </c>
@@ -2376,7 +2373,7 @@
         <v>-6.9600999999999997</v>
       </c>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B5">
         <v>5.4817</v>
       </c>
@@ -2426,7 +2423,7 @@
         <v>9.6417000000000002</v>
       </c>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>-2.5373000000000001</v>
       </c>
@@ -2476,7 +2473,7 @@
         <v>-2.7947000000000002</v>
       </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
         <v>29</v>
       </c>
@@ -2497,7 +2494,7 @@
       </c>
       <c r="P8" s="2"/>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B9" cm="1">
         <f t="array" ref="B9:G13">MMULT(O2:S6,B2:G6)</f>
         <v>92.931623439999996</v>
@@ -2538,7 +2535,7 @@
         <v>35.516657280000004</v>
       </c>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B10">
         <v>67.859226020000008</v>
       </c>
@@ -2576,7 +2573,7 @@
         <v>126.18140964</v>
       </c>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B11">
         <v>-39.116454349999998</v>
       </c>
@@ -2614,7 +2611,7 @@
         <v>402.88913587000002</v>
       </c>
     </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B12">
         <v>-89.784851750000001</v>
       </c>
@@ -2652,7 +2649,7 @@
         <v>-17.671533749999998</v>
       </c>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B13">
         <v>-21.988464449999999</v>
       </c>
@@ -2690,7 +2687,7 @@
         <v>-62.393180920000006</v>
       </c>
     </row>
-    <row r="22" spans="1:831" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:831" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -2701,7 +2698,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:831" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:831" x14ac:dyDescent="0.35">
       <c r="B23">
         <v>1</v>
       </c>
@@ -6022,7 +6019,7 @@
         <v>5.6511623072016253</v>
       </c>
     </row>
-    <row r="24" spans="1:831" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:831" x14ac:dyDescent="0.35">
       <c r="B24">
         <v>1</v>
       </c>
@@ -8514,7 +8511,7 @@
         <v>-2.0406420761190263</v>
       </c>
     </row>
-    <row r="25" spans="1:831" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:831" x14ac:dyDescent="0.35">
       <c r="B25">
         <v>1</v>
       </c>
@@ -11006,7 +11003,7 @@
         <v>-5.6812074243507507</v>
       </c>
     </row>
-    <row r="26" spans="1:831" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:831" x14ac:dyDescent="0.35">
       <c r="B26">
         <v>1</v>
       </c>
@@ -13498,7 +13495,7 @@
         <v>0.83229221322755886</v>
       </c>
     </row>
-    <row r="27" spans="1:831" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:831" x14ac:dyDescent="0.35">
       <c r="B27">
         <v>1</v>
       </c>
@@ -15990,7 +15987,7 @@
         <v>-6.838652432134193</v>
       </c>
     </row>
-    <row r="29" spans="1:831" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:831" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>19</v>
       </c>
@@ -19315,7 +19312,7 @@
         <v>2.2048030018595455E-5</v>
       </c>
     </row>
-    <row r="30" spans="1:831" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:831" x14ac:dyDescent="0.35">
       <c r="B30">
         <v>1213.6230335000002</v>
       </c>
@@ -21807,7 +21804,7 @@
         <v>-8.6543923316639848E-5</v>
       </c>
     </row>
-    <row r="31" spans="1:831" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:831" x14ac:dyDescent="0.35">
       <c r="B31">
         <v>-1634.2809776500003</v>
       </c>
@@ -24299,7 +24296,7 @@
         <v>3.284839226580516E-5</v>
       </c>
     </row>
-    <row r="32" spans="1:831" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:831" x14ac:dyDescent="0.35">
       <c r="B32">
         <v>-81.333507469999972</v>
       </c>
@@ -26791,7 +26788,7 @@
         <v>2.0526255440245222E-5</v>
       </c>
     </row>
-    <row r="33" spans="1:831" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:831" x14ac:dyDescent="0.35">
       <c r="B33">
         <v>-1119.3011452199999</v>
       </c>
@@ -29283,7 +29280,7 @@
         <v>-1.9850137732646544E-5</v>
       </c>
     </row>
-    <row r="35" spans="1:831" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:831" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>16</v>
       </c>
@@ -32608,7 +32605,7 @@
         <v>9.8703382955887686E-9</v>
       </c>
     </row>
-    <row r="37" spans="1:831" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:831" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>17</v>
       </c>
@@ -35933,7 +35930,7 @@
         <v>-6.5152298200788893E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:831" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:831" x14ac:dyDescent="0.35">
       <c r="B38">
         <v>437148.46473176498</v>
       </c>
@@ -38425,7 +38422,7 @@
         <v>-1.0259872494550487E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:831" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:831" x14ac:dyDescent="0.35">
       <c r="B39">
         <v>-461798.20654103038</v>
       </c>
@@ -40917,7 +40914,7 @@
         <v>8.9341976471884049E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:831" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:831" x14ac:dyDescent="0.35">
       <c r="B40">
         <v>-34883.150731436835</v>
       </c>
@@ -43409,7 +43406,7 @@
         <v>3.7148161078850569E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:831" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:831" x14ac:dyDescent="0.35">
       <c r="B41">
         <v>-379648.42332959</v>
       </c>
@@ -45901,7 +45898,7 @@
         <v>8.1481221164322534E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:831" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:831" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>18</v>
       </c>
@@ -49226,7 +49223,7 @@
         <v>9.5226558272119292E-7</v>
       </c>
     </row>
-    <row r="45" spans="1:831" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:831" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>21</v>
       </c>
@@ -52551,7 +52548,7 @@
         <v>1.0365110820642391E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:831" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:831" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>22</v>
       </c>
@@ -55876,7 +55873,7 @@
         <v>9.9349576222492099E-5</v>
       </c>
     </row>
-    <row r="49" spans="1:831" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:831" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>23</v>
       </c>
@@ -59199,6 +59196,11 @@
       <c r="AEY49">
         <f t="shared" si="99"/>
         <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:831" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -59218,17 +59220,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26E0D75C-7C29-445D-9B57-3C648AE105CB}">
   <dimension ref="A1:M52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="1" max="1" width="10.26953125" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>26</v>
       </c>
@@ -59245,7 +59247,7 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B2">
         <v>5.2403000000000004</v>
       </c>
@@ -59280,7 +59282,7 @@
         <v>-2.5373000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B3">
         <v>-1.4360999999999999</v>
       </c>
@@ -59315,7 +59317,7 @@
         <v>2.5573000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>5.1886000000000001</v>
       </c>
@@ -59350,7 +59352,7 @@
         <v>-6.9600999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B5">
         <v>5.4817</v>
       </c>
@@ -59385,7 +59387,7 @@
         <v>9.6417000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>-2.5373000000000001</v>
       </c>
@@ -59420,7 +59422,7 @@
         <v>-2.7947000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
         <v>29</v>
       </c>
@@ -59430,7 +59432,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B9" cm="1">
         <f t="array" ref="B9:G13">MMULT(I2:M6,B2:G6)</f>
         <v>92.931623439999996</v>
@@ -59451,7 +59453,7 @@
         <v>684.5682414900001</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B10">
         <v>67.859226020000008</v>
       </c>
@@ -59471,7 +59473,7 @@
         <v>1222.1996268400003</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B11">
         <v>-39.116454349999998</v>
       </c>
@@ -59491,7 +59493,7 @@
         <v>-1527.2914593500002</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B12">
         <v>-89.784851750000001</v>
       </c>
@@ -59511,7 +59513,7 @@
         <v>-1.6643765899999607</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B13">
         <v>-21.988464449999999</v>
       </c>
@@ -59531,7 +59533,7 @@
         <v>-1088.8854223399999</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -59554,7 +59556,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -59583,7 +59585,7 @@
         <v>-1.5631940186722204E-10</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B18">
         <v>1213.6230335000002</v>
       </c>
@@ -59603,7 +59605,7 @@
         <v>-2.02817318495363E-10</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B19">
         <v>-1634.2809776500003</v>
       </c>
@@ -59623,7 +59625,7 @@
         <v>1.6461854102090001E-10</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B20">
         <v>-81.333507469999972</v>
       </c>
@@ -59643,7 +59645,7 @@
         <v>1.3181988833821379E-10</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B21">
         <v>-1119.3011452199999</v>
       </c>
@@ -59663,7 +59665,7 @@
         <v>1.5188561519607902E-10</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -59688,7 +59690,7 @@
         <v>8.4947297712457903</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C24">
         <f>B18</f>
         <v>1213.6230335000002</v>
@@ -59706,7 +59708,7 @@
         <v>-10.845911521045441</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C25">
         <f>B19</f>
         <v>-1634.2809776500003</v>
@@ -59724,7 +59726,7 @@
         <v>1.1453654923784302</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C26">
         <f>B20</f>
         <v>-81.333507469999972</v>
@@ -59742,7 +59744,7 @@
         <v>1.9420923240793702</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C27">
         <f>B21</f>
         <v>-1119.3011452199999</v>
@@ -59760,36 +59762,36 @@
         <v>-8.6701536509989001</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>36</v>
       </c>
       <c r="B29">
-        <f>B17*B17 + B18*B18 +B19*B19 + B20*B20 + B21*B21</f>
+        <f t="shared" ref="B29:G29" si="0">B17*B17 + B18*B18 +B19*B19 + B20*B20 + B21*B21</f>
         <v>5858381.154742308</v>
       </c>
       <c r="C29">
-        <f>C17*C17 + C18*C18 +C19*C19 + C20*C20 + C21*C21</f>
+        <f t="shared" si="0"/>
         <v>71094.65024840823</v>
       </c>
       <c r="D29">
-        <f>D17*D17 + D18*D18 +D19*D19 + D20*D20 + D21*D21</f>
+        <f t="shared" si="0"/>
         <v>17557.449081013379</v>
       </c>
       <c r="E29">
-        <f>E17*E17 + E18*E18 +E19*E19 + E20*E20 + E21*E21</f>
+        <f t="shared" si="0"/>
         <v>2581.0971895862767</v>
       </c>
       <c r="F29">
-        <f>F17*F17 + F18*F18 +F19*F19 + F20*F20 + F21*F21</f>
+        <f t="shared" si="0"/>
         <v>242.97388399874654</v>
       </c>
       <c r="G29">
-        <f>G17*G17 + G18*G18 +G19*G19 + G20*G20 + G21*G21</f>
+        <f t="shared" si="0"/>
         <v>1.3311560719461585E-19</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>38</v>
       </c>
@@ -59814,7 +59816,7 @@
         <v>24.904123958488128</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C32">
         <v>437148.46473176498</v>
       </c>
@@ -59831,7 +59833,7 @@
         <v>-19.776620458315847</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C33">
         <v>-461798.20654103038</v>
       </c>
@@ -59848,7 +59850,7 @@
         <v>2.8225986710752977</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C34">
         <v>-34883.150731436835</v>
       </c>
@@ -59865,7 +59867,7 @@
         <v>7.8149754320703266</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C35">
         <v>-379648.42332959</v>
       </c>
@@ -59882,7 +59884,7 @@
         <v>-11.121141257383783</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>35</v>
       </c>
@@ -59907,7 +59909,7 @@
         <v>540.88159328531151</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>34</v>
       </c>
@@ -59932,7 +59934,7 @@
         <v>0.44921825222952155</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>33</v>
       </c>
@@ -59957,7 +59959,7 @@
         <v>5.4785973292217108E-22</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>32</v>
       </c>
@@ -59985,7 +59987,7 @@
         <v>5.6511834319749745</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B45">
         <v>1</v>
       </c>
@@ -60005,7 +60007,7 @@
         <v>-2.0406700995792226</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B46">
         <v>1</v>
       </c>
@@ -60025,7 +60027,7 @@
         <v>-5.6812045089773795</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B47">
         <v>1</v>
       </c>
@@ -60045,7 +60047,7 @@
         <v>0.83229689667101359</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B48">
         <v>1</v>
       </c>
@@ -60065,36 +60067,36 @@
         <v>-6.8386749475931659</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>22</v>
       </c>
       <c r="B50">
-        <f>SQRT(B17^2 + B18^2 + B19^2 + B20^2 + B21^2)</f>
+        <f t="shared" ref="B50:G50" si="1">SQRT(B17^2 + B18^2 + B19^2 + B20^2 + B21^2)</f>
         <v>2420.4092948801672</v>
       </c>
       <c r="C50">
-        <f>SQRT(C17^2 + C18^2 + C19^2 + C20^2 + C21^2)</f>
+        <f t="shared" si="1"/>
         <v>266.63580076277873</v>
       </c>
       <c r="D50">
-        <f>SQRT(D17^2 + D18^2 + D19^2 + D20^2 + D21^2)</f>
+        <f t="shared" si="1"/>
         <v>132.50452475675456</v>
       </c>
       <c r="E50">
-        <f>SQRT(E17^2 + E18^2 + E19^2 + E20^2 + E21^2)</f>
+        <f t="shared" si="1"/>
         <v>50.804499698218429</v>
       </c>
       <c r="F50">
-        <f>SQRT(F17^2 + F18^2 + F19^2 + F20^2 + F21^2)</f>
+        <f t="shared" si="1"/>
         <v>15.587619574481106</v>
       </c>
       <c r="G50">
-        <f>SQRT(G17^2 + G18^2 + G19^2 + G20^2 + G21^2)</f>
+        <f t="shared" si="1"/>
         <v>3.6485011606770233E-10</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>39</v>
       </c>
@@ -60107,19 +60109,19 @@
         <v>0</v>
       </c>
       <c r="D52">
-        <f t="shared" ref="D52:E52" si="0">IF(D50 &lt; 0.000001, 1, 0)</f>
+        <f t="shared" ref="D52:E52" si="2">IF(D50 &lt; 0.000001, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="E52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F52">
-        <f t="shared" ref="F52:G52" si="1">IF(F50 &lt; 0.000001, 1, 0)</f>
+        <f t="shared" ref="F52:G52" si="3">IF(F50 &lt; 0.000001, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="G52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>